<commit_message>
#53 03-project-management-playground/01-PMFUPM/Chapter04-Planning/02-create-a-project-schedule/03-work-and-duration-example.xlsx filling in the missing Work hours, Duration, Start Date, End date
</commit_message>
<xml_diff>
--- a/03-project-management-playground/01-PMFUPM/Chapter04-Planning/02-create-a-project-schedule/03-work-and-duration-example.xlsx
+++ b/03-project-management-playground/01-PMFUPM/Chapter04-Planning/02-create-a-project-schedule/03-work-and-duration-example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karlxu/Workspace/github/xuyuji9000/miscellaneous-playground/03-project-management-playground/01-PMFUPM/Chapter04-Planning/02-create-a-project-schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7967756F-A927-B041-88E1-DEEA306E55C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4712BF4B-6D50-BD46-A2DD-57DBD03CD42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17180" xr2:uid="{D0236691-3BAF-4D40-8E5D-E0827B959F17}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
   <si>
     <t>STATUS</t>
   </si>
@@ -174,6 +174,84 @@
   <si>
     <t>END 
 DATE</t>
+  </si>
+  <si>
+    <t>1st Oct</t>
+  </si>
+  <si>
+    <t>7th Nov</t>
+  </si>
+  <si>
+    <t>2nd Nov</t>
+  </si>
+  <si>
+    <t>3rd Nov</t>
+  </si>
+  <si>
+    <t>38 days</t>
+  </si>
+  <si>
+    <t>33 days</t>
+  </si>
+  <si>
+    <t>3 days</t>
+  </si>
+  <si>
+    <t>2 days</t>
+  </si>
+  <si>
+    <t>4th Oct</t>
+  </si>
+  <si>
+    <t>5th Oct</t>
+  </si>
+  <si>
+    <t>4 days</t>
+  </si>
+  <si>
+    <t>6th Oct</t>
+  </si>
+  <si>
+    <t>9th Oct</t>
+  </si>
+  <si>
+    <t>10th Oct</t>
+  </si>
+  <si>
+    <t>12th Oct</t>
+  </si>
+  <si>
+    <t>20th Oct</t>
+  </si>
+  <si>
+    <t>25 days</t>
+  </si>
+  <si>
+    <t>13th Oct</t>
+  </si>
+  <si>
+    <t>5 days</t>
+  </si>
+  <si>
+    <t>17th Oct</t>
+  </si>
+  <si>
+    <t>18th Oct</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>6th Nov</t>
+  </si>
+  <si>
+    <t>10 days</t>
+  </si>
+  <si>
+    <t>19th Oct</t>
+  </si>
+  <si>
+    <t>6 days</t>
   </si>
 </sst>
 </file>
@@ -354,9 +432,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -365,16 +442,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -384,11 +458,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -724,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239A717F-CF11-E14E-955A-EF8DEA678602}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="177" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -736,289 +834,420 @@
     <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12"/>
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8"/>
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="E2" s="12">
+        <v>248</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="E3" s="13">
+        <v>116</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="8"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="E4" s="14">
+        <v>24</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="E5" s="14">
+        <v>6</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="E6" s="14">
+        <v>6</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="E7" s="14">
         <v>16</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
+      <c r="F7" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="E8" s="14">
+        <v>8</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="E9" s="15">
+        <v>56</v>
+      </c>
+      <c r="F9" s="15">
+        <v>14</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="E10" s="13">
+        <v>32</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="E11" s="14">
+        <v>16</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="E12" s="14">
+        <v>8</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="E13" s="14">
+        <v>2</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="E14" s="14">
+        <v>6</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="E15" s="13">
+        <v>36</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="8"/>
+      <c r="E16" s="14">
+        <v>16</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="8"/>
+      <c r="E17" s="14">
+        <v>8</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="8"/>
+      <c r="E18" s="14">
+        <v>4</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10" t="s">
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="11"/>
+      <c r="E19" s="15">
+        <v>8</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>41</v>
+      </c>
+      <c r="E20" s="19">
+        <v>34</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>